<commit_message>
Added an unique ID column to identify regions in production data
</commit_message>
<xml_diff>
--- a/DATA/ProductivityData/Olive_ProductionSurface_Andalusia_2010_2014.xlsx
+++ b/DATA/ProductivityData/Olive_ProductionSurface_Andalusia_2010_2014.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="13">
   <si>
     <t>GRANADA</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>PROVINCE</t>
+  </si>
+  <si>
+    <t>PID</t>
   </si>
 </sst>
 </file>
@@ -107,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -119,60 +122,28 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -184,21 +155,42 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="thin">
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -208,26 +200,100 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
       <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -242,49 +308,49 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -568,590 +634,713 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D41"/>
+  <dimension ref="A1:E41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="24" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5703125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.140625" style="1"/>
+    <col min="1" max="2" width="9.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+    <row r="1" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="D1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="E1" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+    <row r="2" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7">
         <v>2010</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="6">
+      <c r="D2" s="8">
         <v>6961</v>
       </c>
-      <c r="D2" s="7">
+      <c r="E2" s="9">
         <v>64419</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
         <v>2011</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="3">
+      <c r="D3" s="2">
         <v>6961</v>
       </c>
-      <c r="D3" s="4">
+      <c r="E3" s="11">
         <v>51975</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="10">
         <v>2012</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="2">
+        <v>1</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="3">
+      <c r="D4" s="2">
         <v>6961</v>
       </c>
-      <c r="D4" s="4">
+      <c r="E4" s="11">
         <v>51352</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+    <row r="5" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="10">
         <v>2013</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="3">
+      <c r="D5" s="2">
         <v>6893</v>
       </c>
-      <c r="D5" s="4">
+      <c r="E5" s="11">
         <v>50582</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="8">
+    <row r="6" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="12">
         <v>2014</v>
       </c>
-      <c r="B6" s="9" t="s">
+      <c r="B6" s="13">
+        <v>1</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="9">
+      <c r="D6" s="13">
         <v>6896</v>
       </c>
-      <c r="D6" s="10">
+      <c r="E6" s="14">
         <v>53886</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
+    <row r="7" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="7">
         <v>2010</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="8">
+        <v>2</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="6">
+      <c r="D7" s="8">
         <v>21117</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="9">
         <v>37925</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
+    <row r="8" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
         <v>2011</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="2">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="3">
+      <c r="D8" s="2">
         <v>21390</v>
       </c>
-      <c r="D8" s="4">
+      <c r="E8" s="11">
         <v>38163</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
+    <row r="9" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
         <v>2012</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="2">
+        <v>2</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3">
+      <c r="D9" s="2">
         <v>21791</v>
       </c>
-      <c r="D9" s="4">
+      <c r="E9" s="11">
         <v>38152</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
+    <row r="10" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
         <v>2013</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="3">
+      <c r="D10" s="2">
         <v>21390</v>
       </c>
-      <c r="D10" s="4">
+      <c r="E10" s="11">
         <v>47613</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="8">
+    <row r="11" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="12">
         <v>2014</v>
       </c>
-      <c r="B11" s="13" t="s">
+      <c r="B11" s="13">
+        <v>2</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="9">
+      <c r="D11" s="13">
         <v>21390</v>
       </c>
-      <c r="D11" s="10">
+      <c r="E11" s="14">
         <v>44521</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
+    <row r="12" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="7">
         <v>2010</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="8">
+        <v>3</v>
+      </c>
+      <c r="C12" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="6">
+      <c r="D12" s="8">
         <v>322840</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E12" s="9">
         <v>1382695</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
+    <row r="13" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
         <v>2011</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="2">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3">
+      <c r="D13" s="2">
         <v>295016</v>
       </c>
-      <c r="D13" s="4">
+      <c r="E13" s="11">
         <v>1567705</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
+    <row r="14" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
         <v>2012</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="2">
+        <v>3</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="3">
+      <c r="D14" s="2">
         <v>293723</v>
       </c>
-      <c r="D14" s="4">
+      <c r="E14" s="11">
         <v>790786</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+    <row r="15" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
         <v>2013</v>
       </c>
-      <c r="B15" s="12" t="s">
+      <c r="B15" s="2">
+        <v>3</v>
+      </c>
+      <c r="C15" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="3">
+      <c r="D15" s="2">
         <v>294228</v>
       </c>
-      <c r="D15" s="4">
+      <c r="E15" s="11">
         <v>1923154</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="8">
+    <row r="16" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="12">
         <v>2014</v>
       </c>
-      <c r="B16" s="13" t="s">
+      <c r="B16" s="13">
+        <v>3</v>
+      </c>
+      <c r="C16" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="C16" s="9">
+      <c r="D16" s="13">
         <v>294640</v>
       </c>
-      <c r="D16" s="10">
+      <c r="E16" s="14">
         <v>856049</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
+    <row r="17" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="7">
         <v>2010</v>
       </c>
-      <c r="B17" s="11" t="s">
+      <c r="B17" s="8">
+        <v>4</v>
+      </c>
+      <c r="C17" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="6">
+      <c r="D17" s="8">
         <v>145654</v>
       </c>
-      <c r="D17" s="7">
+      <c r="E17" s="9">
         <v>507766</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+    <row r="18" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
         <v>2011</v>
       </c>
-      <c r="B18" s="12" t="s">
+      <c r="B18" s="2">
+        <v>4</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="3">
+      <c r="D18" s="2">
         <v>120998</v>
       </c>
-      <c r="D18" s="4">
+      <c r="E18" s="11">
         <v>673467</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+    <row r="19" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="10">
         <v>2012</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="2">
+        <v>4</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C19" s="3">
+      <c r="D19" s="2">
         <v>121297</v>
       </c>
-      <c r="D19" s="4">
+      <c r="E19" s="11">
         <v>259084</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+    <row r="20" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="10">
         <v>2013</v>
       </c>
-      <c r="B20" s="12" t="s">
+      <c r="B20" s="2">
+        <v>4</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C20" s="3">
+      <c r="D20" s="2">
         <v>118626</v>
       </c>
-      <c r="D20" s="4">
+      <c r="E20" s="11">
         <v>687462</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="8">
+    <row r="21" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="12">
         <v>2014</v>
       </c>
-      <c r="B21" s="13" t="s">
+      <c r="B21" s="13">
+        <v>4</v>
+      </c>
+      <c r="C21" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C21" s="9">
+      <c r="D21" s="13">
         <v>119505</v>
       </c>
-      <c r="D21" s="10">
+      <c r="E21" s="14">
         <v>431583</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="5">
+    <row r="22" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="7">
         <v>2010</v>
       </c>
-      <c r="B22" s="11" t="s">
+      <c r="B22" s="8">
+        <v>5</v>
+      </c>
+      <c r="C22" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="C22" s="6">
+      <c r="D22" s="8">
         <v>28695</v>
       </c>
-      <c r="D22" s="7">
+      <c r="E22" s="9">
         <v>39691</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+    <row r="23" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="10">
         <v>2011</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="2">
+        <v>5</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C23" s="3">
+      <c r="D23" s="2">
         <v>28493</v>
       </c>
-      <c r="D23" s="4">
+      <c r="E23" s="11">
         <v>34607</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
+    <row r="24" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="10">
         <v>2012</v>
       </c>
-      <c r="B24" s="12" t="s">
+      <c r="B24" s="2">
+        <v>5</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C24" s="3">
+      <c r="D24" s="2">
         <v>27730</v>
       </c>
-      <c r="D24" s="4">
+      <c r="E24" s="11">
         <v>30529</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
+    <row r="25" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="10">
         <v>2013</v>
       </c>
-      <c r="B25" s="12" t="s">
+      <c r="B25" s="2">
+        <v>5</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="3">
+      <c r="D25" s="2">
         <v>27228</v>
       </c>
-      <c r="D25" s="4">
+      <c r="E25" s="11">
         <v>31236</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="8">
+    <row r="26" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="12">
         <v>2014</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B26" s="13">
+        <v>5</v>
+      </c>
+      <c r="C26" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="9">
+      <c r="D26" s="13">
         <v>27274</v>
       </c>
-      <c r="D26" s="10">
+      <c r="E26" s="14">
         <v>39814</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+    <row r="27" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="7">
         <v>2010</v>
       </c>
-      <c r="B27" s="11" t="s">
+      <c r="B27" s="8">
+        <v>6</v>
+      </c>
+      <c r="C27" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="6">
+      <c r="D27" s="8">
         <v>387483</v>
       </c>
-      <c r="D27" s="7">
+      <c r="E27" s="9">
         <v>2749955</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+    <row r="28" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="10">
         <v>2011</v>
       </c>
-      <c r="B28" s="12" t="s">
+      <c r="B28" s="2">
+        <v>6</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="3">
+      <c r="D28" s="2">
         <v>310039</v>
       </c>
-      <c r="D28" s="4">
+      <c r="E28" s="11">
         <v>3038311</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+    <row r="29" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="10">
         <v>2012</v>
       </c>
-      <c r="B29" s="12" t="s">
+      <c r="B29" s="2">
+        <v>6</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="3">
+      <c r="D29" s="2">
         <v>310207</v>
       </c>
-      <c r="D29" s="4">
+      <c r="E29" s="11">
         <v>696488</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+    <row r="30" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="10">
         <v>2013</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="2">
+        <v>6</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="3">
+      <c r="D30" s="2">
         <v>310929</v>
       </c>
-      <c r="D30" s="4">
+      <c r="E30" s="11">
         <v>3600871</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="8">
+    <row r="31" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="12">
         <v>2014</v>
       </c>
-      <c r="B31" s="13" t="s">
+      <c r="B31" s="13">
+        <v>6</v>
+      </c>
+      <c r="C31" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="9">
+      <c r="D31" s="13">
         <v>311865</v>
       </c>
-      <c r="D31" s="10">
+      <c r="E31" s="14">
         <v>1023103</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
+    <row r="32" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="7">
         <v>2010</v>
       </c>
-      <c r="B32" s="11" t="s">
+      <c r="B32" s="8">
+        <v>7</v>
+      </c>
+      <c r="C32" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C32" s="6">
+      <c r="D32" s="8">
         <v>117552</v>
       </c>
-      <c r="D32" s="7">
+      <c r="E32" s="9">
         <v>325544</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+    <row r="33" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="10">
         <v>2011</v>
       </c>
-      <c r="B33" s="12" t="s">
+      <c r="B33" s="2">
+        <v>7</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C33" s="3">
+      <c r="D33" s="2">
         <v>104828</v>
       </c>
-      <c r="D33" s="4">
+      <c r="E33" s="11">
         <v>511809</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+    <row r="34" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="10">
         <v>2012</v>
       </c>
-      <c r="B34" s="12" t="s">
+      <c r="B34" s="2">
+        <v>7</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C34" s="3">
+      <c r="D34" s="2">
         <v>102766</v>
       </c>
-      <c r="D34" s="4">
+      <c r="E34" s="11">
         <v>295192</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+    <row r="35" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="10">
         <v>2013</v>
       </c>
-      <c r="B35" s="12" t="s">
+      <c r="B35" s="2">
+        <v>7</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="3">
+      <c r="D35" s="2">
         <v>102743</v>
       </c>
-      <c r="D35" s="4">
+      <c r="E35" s="11">
         <v>449692</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="8">
+    <row r="36" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="12">
         <v>2014</v>
       </c>
-      <c r="B36" s="13" t="s">
+      <c r="B36" s="13">
+        <v>7</v>
+      </c>
+      <c r="C36" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="C36" s="9">
+      <c r="D36" s="13">
         <v>107749</v>
       </c>
-      <c r="D36" s="10">
+      <c r="E36" s="14">
         <v>360502</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
+    <row r="37" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="7">
         <v>2010</v>
       </c>
-      <c r="B37" s="11" t="s">
+      <c r="B37" s="8">
+        <v>8</v>
+      </c>
+      <c r="C37" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C37" s="6">
+      <c r="D37" s="8">
         <v>153615</v>
       </c>
-      <c r="D37" s="7">
+      <c r="E37" s="9">
         <v>812443</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="2">
+    <row r="38" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="10">
         <v>2011</v>
       </c>
-      <c r="B38" s="12" t="s">
+      <c r="B38" s="2">
+        <v>8</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C38" s="3">
+      <c r="D38" s="2">
         <v>140275</v>
       </c>
-      <c r="D38" s="4">
+      <c r="E38" s="11">
         <v>755856</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2">
+    <row r="39" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="10">
         <v>2012</v>
       </c>
-      <c r="B39" s="12" t="s">
+      <c r="B39" s="2">
+        <v>8</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C39" s="3">
+      <c r="D39" s="2">
         <v>140184</v>
       </c>
-      <c r="D39" s="4">
+      <c r="E39" s="11">
         <v>752703</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2">
+    <row r="40" spans="1:5" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="10">
         <v>2013</v>
       </c>
-      <c r="B40" s="12" t="s">
+      <c r="B40" s="2">
+        <v>8</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C40" s="3">
+      <c r="D40" s="2">
         <v>138436</v>
       </c>
-      <c r="D40" s="4">
+      <c r="E40" s="11">
         <v>889587</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="8">
+    <row r="41" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="12">
         <v>2014</v>
       </c>
-      <c r="B41" s="13" t="s">
+      <c r="B41" s="13">
+        <v>8</v>
+      </c>
+      <c r="C41" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="C41" s="9">
+      <c r="D41" s="13">
         <v>137477</v>
       </c>
-      <c r="D41" s="10">
+      <c r="E41" s="14">
         <v>824155</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Changed input production data
</commit_message>
<xml_diff>
--- a/DATA/ProductivityData/Olive_ProductionSurface_Andalusia_2010_2014.xlsx
+++ b/DATA/ProductivityData/Olive_ProductionSurface_Andalusia_2010_2014.xlsx
@@ -303,7 +303,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -335,22 +335,28 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -642,8 +648,8 @@
   <cols>
     <col min="1" max="2" width="9.85546875" style="1" customWidth="1"/>
     <col min="3" max="3" width="13.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" style="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.7109375" style="18" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="10.140625" style="1"/>
   </cols>
   <sheetData>
@@ -657,7 +663,7 @@
       <c r="C1" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="15" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="6" t="s">
@@ -694,7 +700,7 @@
       <c r="D3" s="2">
         <v>6961</v>
       </c>
-      <c r="E3" s="11">
+      <c r="E3" s="16">
         <v>51975</v>
       </c>
     </row>
@@ -711,7 +717,7 @@
       <c r="D4" s="2">
         <v>6961</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="16">
         <v>51352</v>
       </c>
     </row>
@@ -728,24 +734,24 @@
       <c r="D5" s="2">
         <v>6893</v>
       </c>
-      <c r="E5" s="11">
+      <c r="E5" s="16">
         <v>50582</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="12">
+      <c r="A6" s="11">
         <v>2014</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>1</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="13">
+      <c r="D6" s="12">
         <v>6896</v>
       </c>
-      <c r="E6" s="14">
+      <c r="E6" s="17">
         <v>53886</v>
       </c>
     </row>
@@ -756,7 +762,7 @@
       <c r="B7" s="8">
         <v>2</v>
       </c>
-      <c r="C7" s="15" t="s">
+      <c r="C7" s="13" t="s">
         <v>5</v>
       </c>
       <c r="D7" s="8">
@@ -779,7 +785,7 @@
       <c r="D8" s="2">
         <v>21390</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="16">
         <v>38163</v>
       </c>
     </row>
@@ -796,7 +802,7 @@
       <c r="D9" s="2">
         <v>21791</v>
       </c>
-      <c r="E9" s="11">
+      <c r="E9" s="16">
         <v>38152</v>
       </c>
     </row>
@@ -813,24 +819,24 @@
       <c r="D10" s="2">
         <v>21390</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="16">
         <v>47613</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12">
+      <c r="A11" s="11">
         <v>2014</v>
       </c>
-      <c r="B11" s="13">
+      <c r="B11" s="12">
         <v>2</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="C11" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="D11" s="13">
+      <c r="D11" s="12">
         <v>21390</v>
       </c>
-      <c r="E11" s="14">
+      <c r="E11" s="17">
         <v>44521</v>
       </c>
     </row>
@@ -841,7 +847,7 @@
       <c r="B12" s="8">
         <v>3</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="13" t="s">
         <v>6</v>
       </c>
       <c r="D12" s="8">
@@ -864,7 +870,7 @@
       <c r="D13" s="2">
         <v>295016</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="16">
         <v>1567705</v>
       </c>
     </row>
@@ -881,7 +887,7 @@
       <c r="D14" s="2">
         <v>293723</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="16">
         <v>790786</v>
       </c>
     </row>
@@ -898,24 +904,24 @@
       <c r="D15" s="2">
         <v>294228</v>
       </c>
-      <c r="E15" s="11">
+      <c r="E15" s="16">
         <v>1923154</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="12">
+      <c r="A16" s="11">
         <v>2014</v>
       </c>
-      <c r="B16" s="13">
+      <c r="B16" s="12">
         <v>3</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="D16" s="13">
+      <c r="D16" s="12">
         <v>294640</v>
       </c>
-      <c r="E16" s="14">
+      <c r="E16" s="17">
         <v>856049</v>
       </c>
     </row>
@@ -926,7 +932,7 @@
       <c r="B17" s="8">
         <v>4</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="C17" s="13" t="s">
         <v>0</v>
       </c>
       <c r="D17" s="8">
@@ -949,7 +955,7 @@
       <c r="D18" s="2">
         <v>120998</v>
       </c>
-      <c r="E18" s="11">
+      <c r="E18" s="16">
         <v>673467</v>
       </c>
     </row>
@@ -966,7 +972,7 @@
       <c r="D19" s="2">
         <v>121297</v>
       </c>
-      <c r="E19" s="11">
+      <c r="E19" s="16">
         <v>259084</v>
       </c>
     </row>
@@ -983,24 +989,24 @@
       <c r="D20" s="2">
         <v>118626</v>
       </c>
-      <c r="E20" s="11">
+      <c r="E20" s="16">
         <v>687462</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="12">
+      <c r="A21" s="11">
         <v>2014</v>
       </c>
-      <c r="B21" s="13">
+      <c r="B21" s="12">
         <v>4</v>
       </c>
-      <c r="C21" s="16" t="s">
+      <c r="C21" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="D21" s="13">
+      <c r="D21" s="12">
         <v>119505</v>
       </c>
-      <c r="E21" s="14">
+      <c r="E21" s="17">
         <v>431583</v>
       </c>
     </row>
@@ -1011,7 +1017,7 @@
       <c r="B22" s="8">
         <v>5</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="13" t="s">
         <v>2</v>
       </c>
       <c r="D22" s="8">
@@ -1034,7 +1040,7 @@
       <c r="D23" s="2">
         <v>28493</v>
       </c>
-      <c r="E23" s="11">
+      <c r="E23" s="16">
         <v>34607</v>
       </c>
     </row>
@@ -1051,7 +1057,7 @@
       <c r="D24" s="2">
         <v>27730</v>
       </c>
-      <c r="E24" s="11">
+      <c r="E24" s="16">
         <v>30529</v>
       </c>
     </row>
@@ -1068,24 +1074,24 @@
       <c r="D25" s="2">
         <v>27228</v>
       </c>
-      <c r="E25" s="11">
+      <c r="E25" s="16">
         <v>31236</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="12">
+      <c r="A26" s="11">
         <v>2014</v>
       </c>
-      <c r="B26" s="13">
+      <c r="B26" s="12">
         <v>5</v>
       </c>
-      <c r="C26" s="16" t="s">
+      <c r="C26" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="D26" s="13">
+      <c r="D26" s="12">
         <v>27274</v>
       </c>
-      <c r="E26" s="14">
+      <c r="E26" s="17">
         <v>39814</v>
       </c>
     </row>
@@ -1096,7 +1102,7 @@
       <c r="B27" s="8">
         <v>6</v>
       </c>
-      <c r="C27" s="15" t="s">
+      <c r="C27" s="13" t="s">
         <v>7</v>
       </c>
       <c r="D27" s="8">
@@ -1119,7 +1125,7 @@
       <c r="D28" s="2">
         <v>310039</v>
       </c>
-      <c r="E28" s="11">
+      <c r="E28" s="16">
         <v>3038311</v>
       </c>
     </row>
@@ -1136,7 +1142,7 @@
       <c r="D29" s="2">
         <v>310207</v>
       </c>
-      <c r="E29" s="11">
+      <c r="E29" s="16">
         <v>696488</v>
       </c>
     </row>
@@ -1153,24 +1159,24 @@
       <c r="D30" s="2">
         <v>310929</v>
       </c>
-      <c r="E30" s="11">
+      <c r="E30" s="16">
         <v>3600871</v>
       </c>
     </row>
     <row r="31" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="12">
+      <c r="A31" s="11">
         <v>2014</v>
       </c>
-      <c r="B31" s="13">
+      <c r="B31" s="12">
         <v>6</v>
       </c>
-      <c r="C31" s="16" t="s">
+      <c r="C31" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="D31" s="13">
+      <c r="D31" s="12">
         <v>311865</v>
       </c>
-      <c r="E31" s="14">
+      <c r="E31" s="17">
         <v>1023103</v>
       </c>
     </row>
@@ -1181,7 +1187,7 @@
       <c r="B32" s="8">
         <v>7</v>
       </c>
-      <c r="C32" s="15" t="s">
+      <c r="C32" s="13" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="8">
@@ -1204,7 +1210,7 @@
       <c r="D33" s="2">
         <v>104828</v>
       </c>
-      <c r="E33" s="11">
+      <c r="E33" s="16">
         <v>511809</v>
       </c>
     </row>
@@ -1221,7 +1227,7 @@
       <c r="D34" s="2">
         <v>102766</v>
       </c>
-      <c r="E34" s="11">
+      <c r="E34" s="16">
         <v>295192</v>
       </c>
     </row>
@@ -1238,24 +1244,24 @@
       <c r="D35" s="2">
         <v>102743</v>
       </c>
-      <c r="E35" s="11">
+      <c r="E35" s="16">
         <v>449692</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="12">
+      <c r="A36" s="11">
         <v>2014</v>
       </c>
-      <c r="B36" s="13">
+      <c r="B36" s="12">
         <v>7</v>
       </c>
-      <c r="C36" s="16" t="s">
+      <c r="C36" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="D36" s="13">
+      <c r="D36" s="12">
         <v>107749</v>
       </c>
-      <c r="E36" s="14">
+      <c r="E36" s="17">
         <v>360502</v>
       </c>
     </row>
@@ -1266,7 +1272,7 @@
       <c r="B37" s="8">
         <v>8</v>
       </c>
-      <c r="C37" s="15" t="s">
+      <c r="C37" s="13" t="s">
         <v>1</v>
       </c>
       <c r="D37" s="8">
@@ -1289,7 +1295,7 @@
       <c r="D38" s="2">
         <v>140275</v>
       </c>
-      <c r="E38" s="11">
+      <c r="E38" s="16">
         <v>755856</v>
       </c>
     </row>
@@ -1306,7 +1312,7 @@
       <c r="D39" s="2">
         <v>140184</v>
       </c>
-      <c r="E39" s="11">
+      <c r="E39" s="16">
         <v>752703</v>
       </c>
     </row>
@@ -1323,24 +1329,24 @@
       <c r="D40" s="2">
         <v>138436</v>
       </c>
-      <c r="E40" s="11">
+      <c r="E40" s="16">
         <v>889587</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="24" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="12">
+      <c r="A41" s="11">
         <v>2014</v>
       </c>
-      <c r="B41" s="13">
+      <c r="B41" s="12">
         <v>8</v>
       </c>
-      <c r="C41" s="16" t="s">
+      <c r="C41" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="13">
+      <c r="D41" s="12">
         <v>137477</v>
       </c>
-      <c r="E41" s="14">
+      <c r="E41" s="17">
         <v>824155</v>
       </c>
     </row>

</xml_diff>